<commit_message>
updated table with REST Design
</commit_message>
<xml_diff>
--- a/TIWPR-PROJEKT-2/RESTdesign.xlsx
+++ b/TIWPR-PROJEKT-2/RESTdesign.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26227"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26327"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\janbi\Desktop\POLITECHNIKA\2 stopień - SYSTEMY ROZPROSZONE I CHMUROWE\1 semestr\TIwPR\TIwPR-Projekt\TIWPR-PROJEKT-2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F6802DD5-BE17-48ED-AD83-26B8316E901E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7DA16C10-A752-44DC-BF6E-4A9D43E565BA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="76">
   <si>
     <t>GET</t>
   </si>
@@ -93,21 +93,9 @@
     <t>get information of specific tutle</t>
   </si>
   <si>
-    <t>update data of title</t>
-  </si>
-  <si>
-    <t>/statistics/pieces/{piece}</t>
-  </si>
-  <si>
     <t>get list of genders</t>
   </si>
   <si>
-    <t>get number of moves in each game witch</t>
-  </si>
-  <si>
-    <t>get specific statistics of game</t>
-  </si>
-  <si>
     <t>get basics statistics of games</t>
   </si>
   <si>
@@ -117,9 +105,6 @@
     <t>get list of titles</t>
   </si>
   <si>
-    <t>/statistics/games/{gid}</t>
-  </si>
-  <si>
     <t>get list of games won by color</t>
   </si>
   <si>
@@ -132,12 +117,6 @@
     <t>/players/{id}</t>
   </si>
   <si>
-    <t>/games/color/{c}</t>
-  </si>
-  <si>
-    <t>/games/game/{gid}</t>
-  </si>
-  <si>
     <t>/info/titles/</t>
   </si>
   <si>
@@ -145,6 +124,135 @@
   </si>
   <si>
     <t>update part of title</t>
+  </si>
+  <si>
+    <t>get list of users in system (only ADMIN)</t>
+  </si>
+  <si>
+    <t>login user (get token)</t>
+  </si>
+  <si>
+    <t>register new user (response: token)</t>
+  </si>
+  <si>
+    <t>get list of players by gender</t>
+  </si>
+  <si>
+    <t>/admin/users</t>
+  </si>
+  <si>
+    <t>/admin/**</t>
+  </si>
+  <si>
+    <t>/tournaments</t>
+  </si>
+  <si>
+    <t>add tournament</t>
+  </si>
+  <si>
+    <t>update tournament data</t>
+  </si>
+  <si>
+    <t>delete tournament</t>
+  </si>
+  <si>
+    <t>update specific part of tournament</t>
+  </si>
+  <si>
+    <t>get list of tournaments</t>
+  </si>
+  <si>
+    <t>delete title/x</t>
+  </si>
+  <si>
+    <t>??</t>
+  </si>
+  <si>
+    <t>gotowe</t>
+  </si>
+  <si>
+    <t>/games/{gid}</t>
+  </si>
+  <si>
+    <t>/players/{gender}</t>
+  </si>
+  <si>
+    <t>/tokens</t>
+  </si>
+  <si>
+    <t>/games/{colors/draw}</t>
+  </si>
+  <si>
+    <t>/games/{gid}/statistics</t>
+  </si>
+  <si>
+    <t>get statistics of games</t>
+  </si>
+  <si>
+    <t>/tournaments/{id}</t>
+  </si>
+  <si>
+    <t>get info of tournament</t>
+  </si>
+  <si>
+    <t>/tournaments/{country}</t>
+  </si>
+  <si>
+    <t>get list of tournaments in each country</t>
+  </si>
+  <si>
+    <t>/info/tournaments</t>
+  </si>
+  <si>
+    <t xml:space="preserve">get list of tournaments </t>
+  </si>
+  <si>
+    <t>/admin/users/{id}</t>
+  </si>
+  <si>
+    <t>get specific users data</t>
+  </si>
+  <si>
+    <t>/clubs</t>
+  </si>
+  <si>
+    <t>get list of clubs</t>
+  </si>
+  <si>
+    <t>add club</t>
+  </si>
+  <si>
+    <t>/clubs/{cid}</t>
+  </si>
+  <si>
+    <t>get list of players in each club</t>
+  </si>
+  <si>
+    <t>add user to club</t>
+  </si>
+  <si>
+    <t>edit club</t>
+  </si>
+  <si>
+    <t>delete club</t>
+  </si>
+  <si>
+    <t>edit part of club</t>
+  </si>
+  <si>
+    <t>/clubs/transfer/{user1, user2}</t>
+  </si>
+  <si>
+    <t>transfer players between clubs</t>
+  </si>
+  <si>
+    <t>controller</t>
+  </si>
+  <si>
+    <t>edit user data</t>
+  </si>
+  <si>
+    <t>edit specific user data</t>
   </si>
 </sst>
 </file>
@@ -168,7 +276,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -176,11 +284,31 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="9"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color theme="9"/>
+      </right>
+      <top style="thin">
+        <color theme="9"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
@@ -196,6 +324,15 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -243,8 +380,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{9A5283A2-05C3-4EF9-8218-D054DDCB57C1}" name="Tabela1" displayName="Tabela1" ref="C3:I14" totalsRowShown="0" headerRowDxfId="8" dataDxfId="7">
-  <autoFilter ref="C3:I14" xr:uid="{9A5283A2-05C3-4EF9-8218-D054DDCB57C1}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{9A5283A2-05C3-4EF9-8218-D054DDCB57C1}" name="Tabela1" displayName="Tabela1" ref="C3:I25" totalsRowShown="0" headerRowDxfId="8" dataDxfId="7">
+  <autoFilter ref="C3:I25" xr:uid="{9A5283A2-05C3-4EF9-8218-D054DDCB57C1}"/>
   <tableColumns count="7">
     <tableColumn id="1" xr3:uid="{B72B4811-05CE-4733-A03C-BB4227A33DA3}" name="LP" dataDxfId="6"/>
     <tableColumn id="2" xr3:uid="{37F78098-F01B-4E62-B9BB-FD3F43B7744E}" name="endpoint" dataDxfId="5"/>
@@ -521,26 +658,27 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="C3:K26"/>
+  <dimension ref="C3:K34"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="M8" sqref="M8"/>
+    <sheetView tabSelected="1" topLeftCell="A9" zoomScale="80" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="L16" sqref="L16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="3" max="3" width="6.33203125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="27.77734375" customWidth="1"/>
-    <col min="5" max="5" width="19.33203125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11.88671875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="20.33203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.77734375" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="14.88671875" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="13.44140625" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="14.88671875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="29.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="3:11" x14ac:dyDescent="0.3">
+    <row r="3" spans="3:10" x14ac:dyDescent="0.3">
       <c r="C3" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="D3" s="3" t="s">
         <v>5</v>
@@ -560,8 +698,11 @@
       <c r="I3" s="3" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="4" spans="3:11" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="J3" s="2" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="4" spans="3:10" x14ac:dyDescent="0.3">
       <c r="C4" s="2">
         <v>1</v>
       </c>
@@ -581,18 +722,19 @@
         <v>9</v>
       </c>
       <c r="I4" s="3" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="5" spans="3:11" ht="28.8" x14ac:dyDescent="0.3">
+        <v>9</v>
+      </c>
+      <c r="J4" s="2"/>
+    </row>
+    <row r="5" spans="3:10" ht="28.8" x14ac:dyDescent="0.3">
       <c r="C5" s="2">
         <v>2</v>
       </c>
       <c r="D5" s="5" t="s">
-        <v>35</v>
+        <v>51</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="F5" s="3" t="s">
         <v>9</v>
@@ -606,13 +748,14 @@
       <c r="I5" s="3" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="6" spans="3:11" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="J5" s="2"/>
+    </row>
+    <row r="6" spans="3:10" ht="28.8" x14ac:dyDescent="0.3">
       <c r="C6" s="2">
         <v>3</v>
       </c>
       <c r="D6" s="5" t="s">
-        <v>36</v>
+        <v>48</v>
       </c>
       <c r="E6" s="3" t="s">
         <v>14</v>
@@ -629,111 +772,120 @@
       <c r="I6" s="3" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="7" spans="3:11" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="J6" s="2"/>
+    </row>
+    <row r="7" spans="3:10" x14ac:dyDescent="0.3">
       <c r="C7" s="2">
         <v>4</v>
       </c>
       <c r="D7" s="5" t="s">
-        <v>7</v>
+        <v>52</v>
       </c>
       <c r="E7" s="3" t="s">
-        <v>17</v>
+        <v>53</v>
       </c>
       <c r="F7" s="3" t="s">
-        <v>18</v>
+        <v>9</v>
       </c>
       <c r="G7" s="3" t="s">
-        <v>19</v>
+        <v>9</v>
       </c>
       <c r="H7" s="3" t="s">
-        <v>20</v>
+        <v>9</v>
       </c>
       <c r="I7" s="3" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="8" spans="3:11" ht="28.8" x14ac:dyDescent="0.3">
+        <v>9</v>
+      </c>
+      <c r="J7" s="2"/>
+    </row>
+    <row r="8" spans="3:10" ht="28.8" x14ac:dyDescent="0.3">
       <c r="C8" s="2">
         <v>5</v>
       </c>
       <c r="D8" s="5" t="s">
-        <v>34</v>
+        <v>7</v>
       </c>
       <c r="E8" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="F8" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="G8" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="H8" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="I8" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="J8" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="9" spans="3:10" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="C9" s="2">
+        <v>6</v>
+      </c>
+      <c r="D9" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="F8" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="G8" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="H8" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="I8" s="3" t="s">
+      <c r="E9" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="F9" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="G9" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="H9" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="I9" s="8" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="9" spans="3:11" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="C9" s="2">
-        <v>5</v>
-      </c>
-      <c r="D9" s="5" t="s">
-        <v>37</v>
-      </c>
-      <c r="E9" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="F9" s="3" t="s">
+      <c r="J9" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="10" spans="3:10" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="C10" s="2">
+        <v>7</v>
+      </c>
+      <c r="D10" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="E10" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="F10" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="G10" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="H10" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="I10" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="J10" s="2"/>
+    </row>
+    <row r="11" spans="3:10" x14ac:dyDescent="0.3">
+      <c r="C11" s="2">
         <v>8</v>
       </c>
-      <c r="G9" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="H9" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="I9" s="3" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="10" spans="3:11" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="C10" s="2">
-        <v>6</v>
-      </c>
-      <c r="D10" s="5" t="s">
-        <v>32</v>
-      </c>
-      <c r="E10" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="F10" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="G10" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="H10" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="I10" s="3" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="11" spans="3:11" x14ac:dyDescent="0.3">
-      <c r="C11" s="2">
-        <v>7</v>
-      </c>
       <c r="D11" s="5" t="s">
-        <v>33</v>
+        <v>62</v>
       </c>
       <c r="E11" s="3" t="s">
-        <v>24</v>
+        <v>63</v>
       </c>
       <c r="F11" s="3" t="s">
-        <v>9</v>
+        <v>64</v>
       </c>
       <c r="G11" s="3" t="s">
         <v>9</v>
@@ -744,43 +896,44 @@
       <c r="I11" s="3" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="12" spans="3:11" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="J11" s="2"/>
+    </row>
+    <row r="12" spans="3:10" ht="28.8" x14ac:dyDescent="0.3">
       <c r="C12" s="2">
         <v>9</v>
       </c>
       <c r="D12" s="5" t="s">
-        <v>11</v>
+        <v>65</v>
       </c>
       <c r="E12" s="3" t="s">
-        <v>27</v>
+        <v>66</v>
       </c>
       <c r="F12" s="3" t="s">
-        <v>9</v>
+        <v>67</v>
       </c>
       <c r="G12" s="3" t="s">
-        <v>9</v>
+        <v>68</v>
       </c>
       <c r="H12" s="3" t="s">
-        <v>9</v>
+        <v>69</v>
       </c>
       <c r="I12" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="K12" s="2"/>
-    </row>
-    <row r="13" spans="3:11" ht="28.8" x14ac:dyDescent="0.3">
+        <v>70</v>
+      </c>
+      <c r="J12" s="2"/>
+    </row>
+    <row r="13" spans="3:10" ht="57.6" x14ac:dyDescent="0.3">
       <c r="C13" s="2">
         <v>10</v>
       </c>
       <c r="D13" s="5" t="s">
-        <v>30</v>
+        <v>71</v>
       </c>
       <c r="E13" s="3" t="s">
-        <v>26</v>
+        <v>9</v>
       </c>
       <c r="F13" s="3" t="s">
-        <v>9</v>
+        <v>72</v>
       </c>
       <c r="G13" s="3" t="s">
         <v>9</v>
@@ -791,125 +944,364 @@
       <c r="I13" s="3" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="14" spans="3:11" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="J13" s="2" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="14" spans="3:10" ht="43.2" x14ac:dyDescent="0.3">
       <c r="C14" s="2">
         <v>11</v>
       </c>
       <c r="D14" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="E14" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="F14" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="G14" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="H14" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="I14" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="J14" s="2"/>
+    </row>
+    <row r="15" spans="3:10" x14ac:dyDescent="0.3">
+      <c r="C15" s="2">
+        <v>12</v>
+      </c>
+      <c r="D15" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="E15" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="F15" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="G15" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="H15" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="I15" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="J15" s="2"/>
+    </row>
+    <row r="16" spans="3:10" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="C16" s="2">
+        <v>13</v>
+      </c>
+      <c r="D16" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="E16" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="F16" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="G16" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="H16" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="I16" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="J16" s="2"/>
+    </row>
+    <row r="17" spans="3:11" x14ac:dyDescent="0.3">
+      <c r="C17" s="2">
+        <v>14</v>
+      </c>
+      <c r="D17" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="E17" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="F17" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="G17" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="H17" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="I17" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="J17" s="2"/>
+    </row>
+    <row r="18" spans="3:11" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="C18" s="2">
+        <v>15</v>
+      </c>
+      <c r="D18" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="E18" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="F18" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="G18" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="H18" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="I18" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="J18" s="2"/>
+    </row>
+    <row r="19" spans="3:11" x14ac:dyDescent="0.3">
+      <c r="C19" s="2">
+        <v>16</v>
+      </c>
+      <c r="D19" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="E19" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="F19" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="G19" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="H19" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="I19" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="J19" s="2" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="20" spans="3:11" x14ac:dyDescent="0.3">
+      <c r="C20" s="2">
+        <v>17</v>
+      </c>
+      <c r="D20" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="E20" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="F20" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="G20" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="H20" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="I20" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="J20" s="2"/>
+    </row>
+    <row r="21" spans="3:11" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="C21" s="2">
+        <v>18</v>
+      </c>
+      <c r="D21" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="E21" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="E14" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="F14" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="G14" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="H14" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="I14" s="3" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="15" spans="3:11" x14ac:dyDescent="0.3">
-      <c r="D15" s="1"/>
-      <c r="E15" s="1"/>
-      <c r="F15" s="1"/>
-      <c r="G15" s="1"/>
-      <c r="H15" s="1"/>
-      <c r="I15" s="1"/>
-    </row>
-    <row r="16" spans="3:11" x14ac:dyDescent="0.3">
-      <c r="D16" s="1"/>
-      <c r="E16" s="1"/>
-      <c r="F16" s="1"/>
-      <c r="G16" s="1"/>
-      <c r="H16" s="1"/>
-      <c r="I16" s="1"/>
-    </row>
-    <row r="17" spans="4:9" x14ac:dyDescent="0.3">
-      <c r="D17" s="1"/>
-      <c r="E17" s="1"/>
-      <c r="F17" s="1"/>
-      <c r="G17" s="1"/>
-      <c r="H17" s="1"/>
-      <c r="I17" s="1"/>
-    </row>
-    <row r="18" spans="4:9" x14ac:dyDescent="0.3">
-      <c r="D18" s="1"/>
-      <c r="E18" s="1"/>
-      <c r="F18" s="1"/>
-      <c r="G18" s="1"/>
-      <c r="H18" s="1"/>
-      <c r="I18" s="1"/>
-    </row>
-    <row r="19" spans="4:9" x14ac:dyDescent="0.3">
-      <c r="D19" s="4"/>
-      <c r="E19" s="4"/>
-      <c r="F19" s="4"/>
-      <c r="G19" s="4"/>
-      <c r="H19" s="4"/>
-      <c r="I19" s="4"/>
-    </row>
-    <row r="20" spans="4:9" x14ac:dyDescent="0.3">
-      <c r="D20" s="4"/>
-      <c r="E20" s="4"/>
-      <c r="F20" s="4"/>
-      <c r="G20" s="4"/>
-      <c r="H20" s="4"/>
-      <c r="I20" s="4"/>
-    </row>
-    <row r="21" spans="4:9" x14ac:dyDescent="0.3">
-      <c r="D21" s="4"/>
-      <c r="E21" s="4"/>
-      <c r="F21" s="4"/>
-      <c r="G21" s="4"/>
-      <c r="H21" s="4"/>
-      <c r="I21" s="4"/>
-    </row>
-    <row r="22" spans="4:9" x14ac:dyDescent="0.3">
-      <c r="D22" s="4"/>
-      <c r="E22" s="4"/>
-      <c r="F22" s="4"/>
-      <c r="G22" s="4"/>
-      <c r="H22" s="4"/>
-      <c r="I22" s="4"/>
-    </row>
-    <row r="23" spans="4:9" x14ac:dyDescent="0.3">
-      <c r="D23" s="4"/>
-      <c r="E23" s="4"/>
-      <c r="F23" s="4"/>
-      <c r="G23" s="4"/>
-      <c r="H23" s="4"/>
-      <c r="I23" s="4"/>
-    </row>
-    <row r="24" spans="4:9" x14ac:dyDescent="0.3">
-      <c r="D24" s="4"/>
-      <c r="E24" s="4"/>
-      <c r="F24" s="4"/>
-      <c r="G24" s="4"/>
-      <c r="H24" s="4"/>
-      <c r="I24" s="4"/>
-    </row>
-    <row r="25" spans="4:9" x14ac:dyDescent="0.3">
-      <c r="D25" s="4"/>
-      <c r="E25" s="4"/>
-      <c r="F25" s="4"/>
-      <c r="G25" s="4"/>
-      <c r="H25" s="4"/>
-      <c r="I25" s="4"/>
-    </row>
-    <row r="26" spans="4:9" x14ac:dyDescent="0.3">
-      <c r="D26" s="4"/>
-      <c r="E26" s="4"/>
-      <c r="F26" s="4"/>
-      <c r="G26" s="4"/>
-      <c r="H26" s="4"/>
-      <c r="I26" s="4"/>
+      <c r="F21" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="G21" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="H21" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="I21" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="J21" s="2"/>
+      <c r="K21" s="2"/>
+    </row>
+    <row r="22" spans="3:11" x14ac:dyDescent="0.3">
+      <c r="C22" s="2">
+        <v>19</v>
+      </c>
+      <c r="D22" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="E22" s="3"/>
+      <c r="F22" s="3"/>
+      <c r="G22" s="3"/>
+      <c r="H22" s="3"/>
+      <c r="I22" s="3"/>
+      <c r="J22" s="2"/>
+    </row>
+    <row r="23" spans="3:11" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="C23" s="2">
+        <v>20</v>
+      </c>
+      <c r="D23" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="E23" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="F23" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="G23" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="H23" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="I23" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="J23" s="2"/>
+    </row>
+    <row r="24" spans="3:11" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="C24" s="2">
+        <v>21</v>
+      </c>
+      <c r="D24" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="E24" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="F24" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="G24" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="H24" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="I24" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="J24" s="2"/>
+    </row>
+    <row r="25" spans="3:11" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="C25" s="2">
+        <v>22</v>
+      </c>
+      <c r="D25" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="E25" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="F25" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="G25" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="H25" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="I25" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="J25" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="26" spans="3:11" x14ac:dyDescent="0.3">
+      <c r="D26" s="1"/>
+      <c r="E26" s="1"/>
+      <c r="F26" s="1"/>
+      <c r="G26" s="1"/>
+      <c r="H26" s="1"/>
+      <c r="I26" s="1"/>
+    </row>
+    <row r="27" spans="3:11" x14ac:dyDescent="0.3">
+      <c r="D27" s="4"/>
+      <c r="E27" s="4"/>
+      <c r="F27" s="4"/>
+      <c r="G27" s="4"/>
+      <c r="H27" s="4"/>
+      <c r="I27" s="4"/>
+    </row>
+    <row r="28" spans="3:11" x14ac:dyDescent="0.3">
+      <c r="D28" s="4"/>
+      <c r="E28" s="4"/>
+      <c r="F28" s="4"/>
+      <c r="G28" s="4"/>
+      <c r="H28" s="4"/>
+      <c r="I28" s="4"/>
+    </row>
+    <row r="29" spans="3:11" x14ac:dyDescent="0.3">
+      <c r="D29" s="4"/>
+      <c r="E29" s="4"/>
+      <c r="F29" s="4"/>
+      <c r="G29" s="4"/>
+      <c r="H29" s="4"/>
+      <c r="I29" s="4"/>
+    </row>
+    <row r="30" spans="3:11" x14ac:dyDescent="0.3">
+      <c r="D30" s="4"/>
+      <c r="E30" s="4"/>
+      <c r="F30" s="4"/>
+      <c r="G30" s="4"/>
+      <c r="H30" s="4"/>
+      <c r="I30" s="4"/>
+    </row>
+    <row r="31" spans="3:11" x14ac:dyDescent="0.3">
+      <c r="D31" s="4"/>
+      <c r="E31" s="4"/>
+      <c r="F31" s="4"/>
+      <c r="G31" s="4"/>
+      <c r="H31" s="4"/>
+      <c r="I31" s="4"/>
+    </row>
+    <row r="32" spans="3:11" x14ac:dyDescent="0.3">
+      <c r="D32" s="4"/>
+      <c r="E32" s="4"/>
+      <c r="F32" s="4"/>
+      <c r="G32" s="4"/>
+      <c r="H32" s="4"/>
+      <c r="I32" s="4"/>
+    </row>
+    <row r="33" spans="4:9" x14ac:dyDescent="0.3">
+      <c r="D33" s="4"/>
+      <c r="E33" s="4"/>
+      <c r="F33" s="4"/>
+      <c r="G33" s="4"/>
+      <c r="H33" s="4"/>
+      <c r="I33" s="4"/>
+    </row>
+    <row r="34" spans="4:9" x14ac:dyDescent="0.3">
+      <c r="D34" s="4"/>
+      <c r="E34" s="4"/>
+      <c r="F34" s="4"/>
+      <c r="G34" s="4"/>
+      <c r="H34" s="4"/>
+      <c r="I34" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
added possibility to add Players to specific Clubs, updated excel design
</commit_message>
<xml_diff>
--- a/TIWPR-PROJEKT-2/RESTdesign.xlsx
+++ b/TIWPR-PROJEKT-2/RESTdesign.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26327"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25601"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\janbi\Desktop\POLITECHNIKA\2 stopień - SYSTEMY ROZPROSZONE I CHMUROWE\1 semestr\TIwPR\TIwPR-Projekt\TIWPR-PROJEKT-2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A3799677-822D-444C-BFD9-3E94E26D4033}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3D8637EE-66D0-4FA0-B9A6-4F32F1075101}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1920" yWindow="1920" windowWidth="17280" windowHeight="8880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Arkusz1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="133" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="76">
   <si>
     <t>GET</t>
   </si>
@@ -216,12 +216,6 @@
     <t>/clubs/{cid}</t>
   </si>
   <si>
-    <t>get list of players in each club</t>
-  </si>
-  <si>
-    <t>add user to club</t>
-  </si>
-  <si>
     <t>edit club</t>
   </si>
   <si>
@@ -250,6 +244,15 @@
   </si>
   <si>
     <t>get, post</t>
+  </si>
+  <si>
+    <t>add player to club</t>
+  </si>
+  <si>
+    <t>get information of club, and list of players in club</t>
+  </si>
+  <si>
+    <t>GET/POST</t>
   </si>
 </sst>
 </file>
@@ -657,8 +660,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="C3:K33"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="80" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="J16" sqref="J16"/>
+    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="J12" sqref="J12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -818,7 +821,7 @@
         <v>19</v>
       </c>
       <c r="J8" s="2" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
     </row>
     <row r="9" spans="3:10" ht="28.8" x14ac:dyDescent="0.3">
@@ -892,10 +895,10 @@
         <v>9</v>
       </c>
       <c r="J11" s="2" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="12" spans="3:10" ht="28.8" x14ac:dyDescent="0.3">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="12" spans="3:10" ht="43.2" x14ac:dyDescent="0.3">
       <c r="C12" s="2">
         <v>9</v>
       </c>
@@ -903,46 +906,48 @@
         <v>62</v>
       </c>
       <c r="E12" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="F12" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="G12" s="3" t="s">
         <v>63</v>
       </c>
-      <c r="F12" s="3" t="s">
+      <c r="H12" s="3" t="s">
         <v>64</v>
       </c>
-      <c r="G12" s="3" t="s">
+      <c r="I12" s="3" t="s">
         <v>65</v>
       </c>
-      <c r="H12" s="3" t="s">
-        <v>66</v>
-      </c>
-      <c r="I12" s="3" t="s">
-        <v>67</v>
-      </c>
-      <c r="J12" s="2"/>
+      <c r="J12" s="2" t="s">
+        <v>75</v>
+      </c>
     </row>
     <row r="13" spans="3:10" ht="57.6" x14ac:dyDescent="0.3">
       <c r="C13" s="2">
         <v>10</v>
       </c>
       <c r="D13" s="5" t="s">
+        <v>66</v>
+      </c>
+      <c r="E13" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="F13" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="G13" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="H13" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="I13" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="J13" s="2" t="s">
         <v>68</v>
-      </c>
-      <c r="E13" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="F13" s="3" t="s">
-        <v>69</v>
-      </c>
-      <c r="G13" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="H13" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="I13" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="J13" s="2" t="s">
-        <v>70</v>
       </c>
     </row>
     <row r="14" spans="3:10" ht="43.2" x14ac:dyDescent="0.3">
@@ -1150,7 +1155,9 @@
       <c r="I22" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="J22" s="2"/>
+      <c r="J22" s="2" t="s">
+        <v>71</v>
+      </c>
     </row>
     <row r="23" spans="3:11" ht="28.8" x14ac:dyDescent="0.3">
       <c r="C23" s="2">
@@ -1166,13 +1173,13 @@
         <v>9</v>
       </c>
       <c r="G23" s="3" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="H23" s="3" t="s">
         <v>9</v>
       </c>
       <c r="I23" s="3" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="J23" s="2"/>
     </row>

</xml_diff>

<commit_message>
added endpoint to transfer players between two clubs in one operation
</commit_message>
<xml_diff>
--- a/TIWPR-PROJEKT-2/RESTdesign.xlsx
+++ b/TIWPR-PROJEKT-2/RESTdesign.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\janbi\Desktop\POLITECHNIKA\2 stopień - SYSTEMY ROZPROSZONE I CHMUROWE\1 semestr\TIwPR\TIwPR-Projekt\TIWPR-PROJEKT-2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{16068953-3ED0-42D6-A663-CB7C759D9570}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A3AB018D-BD50-43FC-B157-032A51FD8384}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="384" yWindow="384" windowWidth="17280" windowHeight="8880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Arkusz1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="131" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="65">
   <si>
     <t>GET</t>
   </si>
@@ -144,12 +144,6 @@
     <t>get statistics of games</t>
   </si>
   <si>
-    <t>/info/tournaments</t>
-  </si>
-  <si>
-    <t xml:space="preserve">get list of tournaments </t>
-  </si>
-  <si>
     <t>/admin/users/{id}</t>
   </si>
   <si>
@@ -177,9 +171,6 @@
     <t>edit part of club</t>
   </si>
   <si>
-    <t>/clubs/transfer/{user1, user2}</t>
-  </si>
-  <si>
     <t>transfer players between clubs</t>
   </si>
   <si>
@@ -223,6 +214,12 @@
   </si>
   <si>
     <t>get list of games of the specific player</t>
+  </si>
+  <si>
+    <t>/clubs/transfer/idp1=id1&amp;idp2=id2</t>
+  </si>
+  <si>
+    <t>controller</t>
   </si>
 </sst>
 </file>
@@ -308,7 +305,7 @@
   <cellStyles count="1">
     <cellStyle name="Normalny" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="12">
+  <dxfs count="11">
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -326,16 +323,6 @@
       <fill>
         <patternFill>
           <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
         </patternFill>
       </fill>
     </dxf>
@@ -380,16 +367,16 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{9A5283A2-05C3-4EF9-8218-D054DDCB57C1}" name="Tabela1" displayName="Tabela1" ref="C3:I22" totalsRowShown="0" headerRowDxfId="11" dataDxfId="10">
-  <autoFilter ref="C3:I22" xr:uid="{9A5283A2-05C3-4EF9-8218-D054DDCB57C1}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{9A5283A2-05C3-4EF9-8218-D054DDCB57C1}" name="Tabela1" displayName="Tabela1" ref="C3:I21" totalsRowShown="0" headerRowDxfId="10" dataDxfId="9">
+  <autoFilter ref="C3:I21" xr:uid="{9A5283A2-05C3-4EF9-8218-D054DDCB57C1}"/>
   <tableColumns count="7">
-    <tableColumn id="1" xr3:uid="{B72B4811-05CE-4733-A03C-BB4227A33DA3}" name="LP" dataDxfId="9"/>
-    <tableColumn id="2" xr3:uid="{37F78098-F01B-4E62-B9BB-FD3F43B7744E}" name="endpoint" dataDxfId="8"/>
-    <tableColumn id="3" xr3:uid="{6CE0D21B-2E64-43FB-A8DF-4104A24D4B01}" name="GET" dataDxfId="7"/>
-    <tableColumn id="4" xr3:uid="{C358E3FF-D497-4289-8E7C-EFE8B0BE3375}" name="POST" dataDxfId="6"/>
-    <tableColumn id="5" xr3:uid="{7035C704-2379-47A9-8EED-8B00962C66F6}" name="PUT" dataDxfId="5"/>
-    <tableColumn id="6" xr3:uid="{CAB59842-C01B-47AA-ADB0-BEDA58388076}" name="DELETE" dataDxfId="4"/>
-    <tableColumn id="7" xr3:uid="{55AC5320-F311-42EC-8EE3-50B77673B9EF}" name="PATCH" dataDxfId="3"/>
+    <tableColumn id="1" xr3:uid="{B72B4811-05CE-4733-A03C-BB4227A33DA3}" name="LP" dataDxfId="8"/>
+    <tableColumn id="2" xr3:uid="{37F78098-F01B-4E62-B9BB-FD3F43B7744E}" name="endpoint" dataDxfId="7"/>
+    <tableColumn id="3" xr3:uid="{6CE0D21B-2E64-43FB-A8DF-4104A24D4B01}" name="GET" dataDxfId="6"/>
+    <tableColumn id="4" xr3:uid="{C358E3FF-D497-4289-8E7C-EFE8B0BE3375}" name="POST" dataDxfId="5"/>
+    <tableColumn id="5" xr3:uid="{7035C704-2379-47A9-8EED-8B00962C66F6}" name="PUT" dataDxfId="4"/>
+    <tableColumn id="6" xr3:uid="{CAB59842-C01B-47AA-ADB0-BEDA58388076}" name="DELETE" dataDxfId="3"/>
+    <tableColumn id="7" xr3:uid="{55AC5320-F311-42EC-8EE3-50B77673B9EF}" name="PATCH" dataDxfId="2"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight14" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -658,10 +645,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="C3:K31"/>
+  <dimension ref="C3:K30"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="K8" sqref="K8"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -674,6 +661,7 @@
     <col min="8" max="8" width="13.44140625" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="14.88671875" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="29.88671875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="9.77734375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="3" spans="3:11" x14ac:dyDescent="0.3">
@@ -699,7 +687,7 @@
         <v>4</v>
       </c>
       <c r="J3" s="3" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
     </row>
     <row r="4" spans="3:11" x14ac:dyDescent="0.3">
@@ -725,7 +713,7 @@
         <v>8</v>
       </c>
       <c r="J4" s="2" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
     </row>
     <row r="5" spans="3:11" ht="28.8" x14ac:dyDescent="0.3">
@@ -733,7 +721,7 @@
         <v>2</v>
       </c>
       <c r="D5" s="5" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="E5" s="3" t="s">
         <v>24</v>
@@ -751,7 +739,7 @@
         <v>8</v>
       </c>
       <c r="J5" s="2" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="K5" s="2"/>
     </row>
@@ -805,7 +793,7 @@
         <v>8</v>
       </c>
       <c r="J7" s="2" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="K7" s="2"/>
     </row>
@@ -814,10 +802,10 @@
         <v>5</v>
       </c>
       <c r="D8" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="E8" s="3" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="F8" s="2" t="s">
         <v>8</v>
@@ -832,7 +820,7 @@
         <v>8</v>
       </c>
       <c r="J8" s="2" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="K8" s="2"/>
     </row>
@@ -859,7 +847,7 @@
         <v>18</v>
       </c>
       <c r="J9" s="2" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="K9" s="2"/>
     </row>
@@ -871,7 +859,7 @@
         <v>26</v>
       </c>
       <c r="E10" s="7" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="F10" s="7" t="s">
         <v>8</v>
@@ -886,7 +874,7 @@
         <v>9</v>
       </c>
       <c r="J10" s="2" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="K10" s="2"/>
     </row>
@@ -913,7 +901,7 @@
         <v>8</v>
       </c>
       <c r="J11" s="2" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="K11" s="2"/>
     </row>
@@ -922,14 +910,14 @@
         <v>9</v>
       </c>
       <c r="D12" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="E12" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="F12" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="E12" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="F12" s="3" t="s">
-        <v>45</v>
-      </c>
       <c r="G12" s="3" t="s">
         <v>8</v>
       </c>
@@ -940,7 +928,7 @@
         <v>8</v>
       </c>
       <c r="J12" s="2" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="K12" s="2"/>
     </row>
@@ -949,52 +937,56 @@
         <v>10</v>
       </c>
       <c r="D13" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="E13" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="F13" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="G13" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="H13" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="E13" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="F13" s="3" t="s">
-        <v>55</v>
-      </c>
-      <c r="G13" s="3" t="s">
+      <c r="I13" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="H13" s="3" t="s">
-        <v>48</v>
-      </c>
-      <c r="I13" s="3" t="s">
-        <v>49</v>
-      </c>
       <c r="J13" s="2" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="K13" s="2"/>
     </row>
-    <row r="14" spans="3:11" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="14" spans="3:11" ht="28.8" x14ac:dyDescent="0.3">
       <c r="C14" s="2">
         <v>11</v>
       </c>
       <c r="D14" s="5" t="s">
-        <v>50</v>
+        <v>63</v>
       </c>
       <c r="E14" s="3" t="s">
         <v>8</v>
       </c>
       <c r="F14" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="G14" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="H14" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="I14" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="J14" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="G14" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="H14" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="I14" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="J14" s="2"/>
-      <c r="K14" s="2"/>
+      <c r="K14" s="2" t="s">
+        <v>64</v>
+      </c>
     </row>
     <row r="15" spans="3:11" x14ac:dyDescent="0.3">
       <c r="C15" s="2">
@@ -1019,7 +1011,7 @@
         <v>8</v>
       </c>
       <c r="J15" s="2" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="K15" s="2"/>
     </row>
@@ -1046,19 +1038,19 @@
         <v>8</v>
       </c>
       <c r="J16" s="2" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="K16" s="2"/>
     </row>
-    <row r="17" spans="3:11" x14ac:dyDescent="0.3">
+    <row r="17" spans="3:11" ht="28.8" x14ac:dyDescent="0.3">
       <c r="C17" s="2">
         <v>14</v>
       </c>
       <c r="D17" s="5" t="s">
-        <v>39</v>
+        <v>10</v>
       </c>
       <c r="E17" s="3" t="s">
-        <v>40</v>
+        <v>21</v>
       </c>
       <c r="F17" s="3" t="s">
         <v>8</v>
@@ -1075,71 +1067,71 @@
       <c r="J17" s="2"/>
       <c r="K17" s="2"/>
     </row>
-    <row r="18" spans="3:11" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="18" spans="3:11" x14ac:dyDescent="0.3">
       <c r="C18" s="2">
         <v>15</v>
       </c>
       <c r="D18" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="E18" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="F18" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="G18" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="H18" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="I18" s="3" t="s">
-        <v>8</v>
-      </c>
+        <v>33</v>
+      </c>
+      <c r="E18" s="3"/>
+      <c r="F18" s="3"/>
+      <c r="G18" s="3"/>
+      <c r="H18" s="3"/>
+      <c r="I18" s="3"/>
       <c r="J18" s="2"/>
       <c r="K18" s="2"/>
     </row>
-    <row r="19" spans="3:11" x14ac:dyDescent="0.3">
+    <row r="19" spans="3:11" ht="43.2" x14ac:dyDescent="0.3">
       <c r="C19" s="2">
         <v>16</v>
       </c>
       <c r="D19" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="E19" s="3"/>
-      <c r="F19" s="3"/>
-      <c r="G19" s="3"/>
-      <c r="H19" s="3"/>
-      <c r="I19" s="3"/>
-      <c r="J19" s="2"/>
+        <v>32</v>
+      </c>
+      <c r="E19" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="F19" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="G19" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="H19" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="I19" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="J19" s="2" t="s">
+        <v>51</v>
+      </c>
       <c r="K19" s="2"/>
     </row>
-    <row r="20" spans="3:11" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="20" spans="3:11" ht="28.8" x14ac:dyDescent="0.3">
       <c r="C20" s="2">
         <v>17</v>
       </c>
       <c r="D20" s="5" t="s">
-        <v>32</v>
+        <v>39</v>
       </c>
       <c r="E20" s="3" t="s">
-        <v>28</v>
+        <v>40</v>
       </c>
       <c r="F20" s="3" t="s">
-        <v>30</v>
+        <v>8</v>
       </c>
       <c r="G20" s="3" t="s">
-        <v>8</v>
+        <v>49</v>
       </c>
       <c r="H20" s="3" t="s">
         <v>8</v>
       </c>
       <c r="I20" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="J20" s="2" t="s">
-        <v>54</v>
-      </c>
+        <v>50</v>
+      </c>
+      <c r="J20" s="2"/>
       <c r="K20" s="2"/>
     </row>
     <row r="21" spans="3:11" ht="28.8" x14ac:dyDescent="0.3">
@@ -1147,60 +1139,43 @@
         <v>18</v>
       </c>
       <c r="D21" s="5" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="E21" s="3" t="s">
-        <v>42</v>
+        <v>8</v>
       </c>
       <c r="F21" s="3" t="s">
-        <v>8</v>
+        <v>29</v>
       </c>
       <c r="G21" s="3" t="s">
-        <v>52</v>
+        <v>8</v>
       </c>
       <c r="H21" s="3" t="s">
         <v>8</v>
       </c>
       <c r="I21" s="3" t="s">
-        <v>53</v>
-      </c>
-      <c r="J21" s="2"/>
+        <v>8</v>
+      </c>
+      <c r="J21" s="2" t="s">
+        <v>51</v>
+      </c>
       <c r="K21" s="2"/>
     </row>
-    <row r="22" spans="3:11" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="C22" s="2">
-        <v>19</v>
-      </c>
-      <c r="D22" s="5" t="s">
-        <v>36</v>
-      </c>
-      <c r="E22" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="F22" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="G22" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="H22" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="I22" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="J22" s="2" t="s">
-        <v>54</v>
-      </c>
-      <c r="K22" s="2"/>
+    <row r="22" spans="3:11" x14ac:dyDescent="0.3">
+      <c r="D22" s="1"/>
+      <c r="E22" s="1"/>
+      <c r="F22" s="1"/>
+      <c r="G22" s="1"/>
+      <c r="H22" s="1"/>
+      <c r="I22" s="1"/>
     </row>
     <row r="23" spans="3:11" x14ac:dyDescent="0.3">
-      <c r="D23" s="1"/>
-      <c r="E23" s="1"/>
-      <c r="F23" s="1"/>
-      <c r="G23" s="1"/>
-      <c r="H23" s="1"/>
-      <c r="I23" s="1"/>
+      <c r="D23" s="4"/>
+      <c r="E23" s="4"/>
+      <c r="F23" s="4"/>
+      <c r="G23" s="4"/>
+      <c r="H23" s="4"/>
+      <c r="I23" s="4"/>
     </row>
     <row r="24" spans="3:11" x14ac:dyDescent="0.3">
       <c r="D24" s="4"/>
@@ -1258,16 +1233,8 @@
       <c r="H30" s="4"/>
       <c r="I30" s="4"/>
     </row>
-    <row r="31" spans="3:11" x14ac:dyDescent="0.3">
-      <c r="D31" s="4"/>
-      <c r="E31" s="4"/>
-      <c r="F31" s="4"/>
-      <c r="G31" s="4"/>
-      <c r="H31" s="4"/>
-      <c r="I31" s="4"/>
-    </row>
   </sheetData>
-  <conditionalFormatting sqref="J4:J22">
+  <conditionalFormatting sqref="J4:J21">
     <cfRule type="cellIs" dxfId="1" priority="1" operator="equal">
       <formula>"done"</formula>
     </cfRule>

</xml_diff>

<commit_message>
added possibility to filter players by gender
</commit_message>
<xml_diff>
--- a/TIWPR-PROJEKT-2/RESTdesign.xlsx
+++ b/TIWPR-PROJEKT-2/RESTdesign.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\janbi\Desktop\POLITECHNIKA\2 stopień - SYSTEMY ROZPROSZONE I CHMUROWE\1 semestr\TIwPR\TIwPR-Projekt\TIWPR-PROJEKT-2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A3AB018D-BD50-43FC-B157-032A51FD8384}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B9D0A498-AE1B-409A-B6AE-447DF761F379}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="384" yWindow="384" windowWidth="17280" windowHeight="8880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Arkusz1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="62">
   <si>
     <t>GET</t>
   </si>
@@ -126,15 +126,9 @@
     <t>/admin/users</t>
   </si>
   <si>
-    <t>/admin/**</t>
-  </si>
-  <si>
     <t>/games/{gid}</t>
   </si>
   <si>
-    <t>/players/{gender}</t>
-  </si>
-  <si>
     <t>/tokens</t>
   </si>
   <si>
@@ -204,9 +198,6 @@
     <t>???</t>
   </si>
   <si>
-    <t>??</t>
-  </si>
-  <si>
     <t>Gotowe</t>
   </si>
   <si>
@@ -219,7 +210,7 @@
     <t>/clubs/transfer/idp1=id1&amp;idp2=id2</t>
   </si>
   <si>
-    <t>controller</t>
+    <t>/players?gender={gender}</t>
   </si>
 </sst>
 </file>
@@ -367,8 +358,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{9A5283A2-05C3-4EF9-8218-D054DDCB57C1}" name="Tabela1" displayName="Tabela1" ref="C3:I21" totalsRowShown="0" headerRowDxfId="10" dataDxfId="9">
-  <autoFilter ref="C3:I21" xr:uid="{9A5283A2-05C3-4EF9-8218-D054DDCB57C1}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{9A5283A2-05C3-4EF9-8218-D054DDCB57C1}" name="Tabela1" displayName="Tabela1" ref="C3:I20" totalsRowShown="0" headerRowDxfId="10" dataDxfId="9">
+  <autoFilter ref="C3:I20" xr:uid="{9A5283A2-05C3-4EF9-8218-D054DDCB57C1}"/>
   <tableColumns count="7">
     <tableColumn id="1" xr3:uid="{B72B4811-05CE-4733-A03C-BB4227A33DA3}" name="LP" dataDxfId="8"/>
     <tableColumn id="2" xr3:uid="{37F78098-F01B-4E62-B9BB-FD3F43B7744E}" name="endpoint" dataDxfId="7"/>
@@ -645,10 +636,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="C3:K30"/>
+  <dimension ref="C3:K29"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="K6" sqref="K6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -687,7 +678,7 @@
         <v>4</v>
       </c>
       <c r="J3" s="3" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
     </row>
     <row r="4" spans="3:11" x14ac:dyDescent="0.3">
@@ -713,7 +704,7 @@
         <v>8</v>
       </c>
       <c r="J4" s="2" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
     </row>
     <row r="5" spans="3:11" ht="28.8" x14ac:dyDescent="0.3">
@@ -721,7 +712,7 @@
         <v>2</v>
       </c>
       <c r="D5" s="5" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="E5" s="3" t="s">
         <v>24</v>
@@ -739,7 +730,7 @@
         <v>8</v>
       </c>
       <c r="J5" s="2" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="K5" s="2"/>
     </row>
@@ -748,7 +739,7 @@
         <v>3</v>
       </c>
       <c r="D6" s="5" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E6" s="3" t="s">
         <v>13</v>
@@ -775,10 +766,10 @@
         <v>4</v>
       </c>
       <c r="D7" s="5" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="E7" s="3" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="F7" s="3" t="s">
         <v>8</v>
@@ -793,7 +784,7 @@
         <v>8</v>
       </c>
       <c r="J7" s="2" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="K7" s="2"/>
     </row>
@@ -802,10 +793,10 @@
         <v>5</v>
       </c>
       <c r="D8" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="E8" s="3" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="F8" s="2" t="s">
         <v>8</v>
@@ -820,7 +811,7 @@
         <v>8</v>
       </c>
       <c r="J8" s="2" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="K8" s="2"/>
     </row>
@@ -847,7 +838,7 @@
         <v>18</v>
       </c>
       <c r="J9" s="2" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="K9" s="2"/>
     </row>
@@ -859,7 +850,7 @@
         <v>26</v>
       </c>
       <c r="E10" s="7" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="F10" s="7" t="s">
         <v>8</v>
@@ -874,7 +865,7 @@
         <v>9</v>
       </c>
       <c r="J10" s="2" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="K10" s="2"/>
     </row>
@@ -883,7 +874,7 @@
         <v>8</v>
       </c>
       <c r="D11" s="5" t="s">
-        <v>35</v>
+        <v>61</v>
       </c>
       <c r="E11" s="3" t="s">
         <v>31</v>
@@ -901,7 +892,7 @@
         <v>8</v>
       </c>
       <c r="J11" s="2" t="s">
-        <v>59</v>
+        <v>49</v>
       </c>
       <c r="K11" s="2"/>
     </row>
@@ -910,14 +901,14 @@
         <v>9</v>
       </c>
       <c r="D12" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="E12" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="F12" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="E12" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="F12" s="3" t="s">
-        <v>43</v>
-      </c>
       <c r="G12" s="3" t="s">
         <v>8</v>
       </c>
@@ -928,7 +919,7 @@
         <v>8</v>
       </c>
       <c r="J12" s="2" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="K12" s="2"/>
     </row>
@@ -937,25 +928,25 @@
         <v>10</v>
       </c>
       <c r="D13" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="E13" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="F13" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="G13" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="H13" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="E13" s="3" t="s">
-        <v>53</v>
-      </c>
-      <c r="F13" s="3" t="s">
+      <c r="I13" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="J13" s="2" t="s">
         <v>52</v>
-      </c>
-      <c r="G13" s="3" t="s">
-        <v>45</v>
-      </c>
-      <c r="H13" s="3" t="s">
-        <v>46</v>
-      </c>
-      <c r="I13" s="3" t="s">
-        <v>47</v>
-      </c>
-      <c r="J13" s="2" t="s">
-        <v>54</v>
       </c>
       <c r="K13" s="2"/>
     </row>
@@ -964,13 +955,13 @@
         <v>11</v>
       </c>
       <c r="D14" s="5" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="E14" s="3" t="s">
         <v>8</v>
       </c>
       <c r="F14" s="3" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="G14" s="3" t="s">
         <v>8</v>
@@ -982,11 +973,9 @@
         <v>8</v>
       </c>
       <c r="J14" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="K14" s="2" t="s">
-        <v>64</v>
-      </c>
+        <v>49</v>
+      </c>
+      <c r="K14" s="2"/>
     </row>
     <row r="15" spans="3:11" x14ac:dyDescent="0.3">
       <c r="C15" s="2">
@@ -1011,7 +1000,7 @@
         <v>8</v>
       </c>
       <c r="J15" s="2" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="K15" s="2"/>
     </row>
@@ -1038,7 +1027,7 @@
         <v>8</v>
       </c>
       <c r="J16" s="2" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="K16" s="2"/>
     </row>
@@ -1067,107 +1056,102 @@
       <c r="J17" s="2"/>
       <c r="K17" s="2"/>
     </row>
-    <row r="18" spans="3:11" x14ac:dyDescent="0.3">
+    <row r="18" spans="3:11" ht="43.2" x14ac:dyDescent="0.3">
       <c r="C18" s="2">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D18" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="E18" s="3"/>
-      <c r="F18" s="3"/>
-      <c r="G18" s="3"/>
-      <c r="H18" s="3"/>
-      <c r="I18" s="3"/>
-      <c r="J18" s="2"/>
+        <v>32</v>
+      </c>
+      <c r="E18" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="F18" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="G18" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="H18" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="I18" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="J18" s="2" t="s">
+        <v>49</v>
+      </c>
       <c r="K18" s="2"/>
     </row>
-    <row r="19" spans="3:11" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="19" spans="3:11" ht="28.8" x14ac:dyDescent="0.3">
       <c r="C19" s="2">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="D19" s="5" t="s">
-        <v>32</v>
+        <v>37</v>
       </c>
       <c r="E19" s="3" t="s">
-        <v>28</v>
+        <v>38</v>
       </c>
       <c r="F19" s="3" t="s">
-        <v>30</v>
+        <v>8</v>
       </c>
       <c r="G19" s="3" t="s">
-        <v>8</v>
+        <v>47</v>
       </c>
       <c r="H19" s="3" t="s">
         <v>8</v>
       </c>
       <c r="I19" s="3" t="s">
-        <v>8</v>
+        <v>48</v>
       </c>
       <c r="J19" s="2" t="s">
-        <v>51</v>
+        <v>0</v>
       </c>
       <c r="K19" s="2"/>
     </row>
     <row r="20" spans="3:11" ht="28.8" x14ac:dyDescent="0.3">
       <c r="C20" s="2">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="D20" s="5" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
       <c r="E20" s="3" t="s">
-        <v>40</v>
+        <v>8</v>
       </c>
       <c r="F20" s="3" t="s">
-        <v>8</v>
+        <v>29</v>
       </c>
       <c r="G20" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="H20" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="I20" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="J20" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="H20" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="I20" s="3" t="s">
-        <v>50</v>
-      </c>
-      <c r="J20" s="2"/>
       <c r="K20" s="2"/>
     </row>
-    <row r="21" spans="3:11" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="C21" s="2">
-        <v>18</v>
-      </c>
-      <c r="D21" s="5" t="s">
-        <v>36</v>
-      </c>
-      <c r="E21" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="F21" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="G21" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="H21" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="I21" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="J21" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="K21" s="2"/>
+    <row r="21" spans="3:11" x14ac:dyDescent="0.3">
+      <c r="D21" s="1"/>
+      <c r="E21" s="1"/>
+      <c r="F21" s="1"/>
+      <c r="G21" s="1"/>
+      <c r="H21" s="1"/>
+      <c r="I21" s="1"/>
     </row>
     <row r="22" spans="3:11" x14ac:dyDescent="0.3">
-      <c r="D22" s="1"/>
-      <c r="E22" s="1"/>
-      <c r="F22" s="1"/>
-      <c r="G22" s="1"/>
-      <c r="H22" s="1"/>
-      <c r="I22" s="1"/>
+      <c r="D22" s="4"/>
+      <c r="E22" s="4"/>
+      <c r="F22" s="4"/>
+      <c r="G22" s="4"/>
+      <c r="H22" s="4"/>
+      <c r="I22" s="4"/>
     </row>
     <row r="23" spans="3:11" x14ac:dyDescent="0.3">
       <c r="D23" s="4"/>
@@ -1225,16 +1209,8 @@
       <c r="H29" s="4"/>
       <c r="I29" s="4"/>
     </row>
-    <row r="30" spans="3:11" x14ac:dyDescent="0.3">
-      <c r="D30" s="4"/>
-      <c r="E30" s="4"/>
-      <c r="F30" s="4"/>
-      <c r="G30" s="4"/>
-      <c r="H30" s="4"/>
-      <c r="I30" s="4"/>
-    </row>
   </sheetData>
-  <conditionalFormatting sqref="J4:J21">
+  <conditionalFormatting sqref="J4:J20">
     <cfRule type="cellIs" dxfId="1" priority="1" operator="equal">
       <formula>"done"</formula>
     </cfRule>

</xml_diff>

<commit_message>
added POST once exactly mechanism
</commit_message>
<xml_diff>
--- a/TIWPR-PROJEKT-2/RESTdesign.xlsx
+++ b/TIWPR-PROJEKT-2/RESTdesign.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\janbi\Desktop\POLITECHNIKA\2 stopień - SYSTEMY ROZPROSZONE I CHMUROWE\1 semestr\TIwPR\TIwPR-Projekt\TIWPR-PROJEKT-2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B9D0A498-AE1B-409A-B6AE-447DF761F379}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D63E3D67-841F-4336-8150-665DAC7EC4DD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="63">
   <si>
     <t>GET</t>
   </si>
@@ -195,9 +195,6 @@
     <t>/games?result{WHITE/BLACK/DRAW}</t>
   </si>
   <si>
-    <t>???</t>
-  </si>
-  <si>
     <t>Gotowe</t>
   </si>
   <si>
@@ -211,6 +208,12 @@
   </si>
   <si>
     <t>/players?gender={gender}</t>
+  </si>
+  <si>
+    <t>site in build</t>
+  </si>
+  <si>
+    <t>get token to POST</t>
   </si>
 </sst>
 </file>
@@ -298,26 +301,6 @@
   </cellStyles>
   <dxfs count="11">
     <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
@@ -344,6 +327,26 @@
     <dxf>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -358,16 +361,16 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{9A5283A2-05C3-4EF9-8218-D054DDCB57C1}" name="Tabela1" displayName="Tabela1" ref="C3:I20" totalsRowShown="0" headerRowDxfId="10" dataDxfId="9">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{9A5283A2-05C3-4EF9-8218-D054DDCB57C1}" name="Tabela1" displayName="Tabela1" ref="C3:I20" totalsRowShown="0" headerRowDxfId="8" dataDxfId="7">
   <autoFilter ref="C3:I20" xr:uid="{9A5283A2-05C3-4EF9-8218-D054DDCB57C1}"/>
   <tableColumns count="7">
-    <tableColumn id="1" xr3:uid="{B72B4811-05CE-4733-A03C-BB4227A33DA3}" name="LP" dataDxfId="8"/>
-    <tableColumn id="2" xr3:uid="{37F78098-F01B-4E62-B9BB-FD3F43B7744E}" name="endpoint" dataDxfId="7"/>
-    <tableColumn id="3" xr3:uid="{6CE0D21B-2E64-43FB-A8DF-4104A24D4B01}" name="GET" dataDxfId="6"/>
-    <tableColumn id="4" xr3:uid="{C358E3FF-D497-4289-8E7C-EFE8B0BE3375}" name="POST" dataDxfId="5"/>
-    <tableColumn id="5" xr3:uid="{7035C704-2379-47A9-8EED-8B00962C66F6}" name="PUT" dataDxfId="4"/>
-    <tableColumn id="6" xr3:uid="{CAB59842-C01B-47AA-ADB0-BEDA58388076}" name="DELETE" dataDxfId="3"/>
-    <tableColumn id="7" xr3:uid="{55AC5320-F311-42EC-8EE3-50B77673B9EF}" name="PATCH" dataDxfId="2"/>
+    <tableColumn id="1" xr3:uid="{B72B4811-05CE-4733-A03C-BB4227A33DA3}" name="LP" dataDxfId="6"/>
+    <tableColumn id="2" xr3:uid="{37F78098-F01B-4E62-B9BB-FD3F43B7744E}" name="endpoint" dataDxfId="5"/>
+    <tableColumn id="3" xr3:uid="{6CE0D21B-2E64-43FB-A8DF-4104A24D4B01}" name="GET" dataDxfId="4"/>
+    <tableColumn id="4" xr3:uid="{C358E3FF-D497-4289-8E7C-EFE8B0BE3375}" name="POST" dataDxfId="3"/>
+    <tableColumn id="5" xr3:uid="{7035C704-2379-47A9-8EED-8B00962C66F6}" name="PUT" dataDxfId="2"/>
+    <tableColumn id="6" xr3:uid="{CAB59842-C01B-47AA-ADB0-BEDA58388076}" name="DELETE" dataDxfId="1"/>
+    <tableColumn id="7" xr3:uid="{55AC5320-F311-42EC-8EE3-50B77673B9EF}" name="PATCH" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight14" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -639,7 +642,7 @@
   <dimension ref="C3:K29"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="K6" sqref="K6"/>
+      <selection activeCell="K7" sqref="K7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -652,7 +655,7 @@
     <col min="8" max="8" width="13.44140625" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="14.88671875" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="29.88671875" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="9.77734375" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="11.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="3" spans="3:11" x14ac:dyDescent="0.3">
@@ -678,7 +681,7 @@
         <v>4</v>
       </c>
       <c r="J3" s="3" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="4" spans="3:11" x14ac:dyDescent="0.3">
@@ -784,19 +787,21 @@
         <v>8</v>
       </c>
       <c r="J7" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="K7" s="2"/>
+        <v>49</v>
+      </c>
+      <c r="K7" s="2" t="s">
+        <v>61</v>
+      </c>
     </row>
     <row r="8" spans="3:11" ht="28.8" x14ac:dyDescent="0.3">
       <c r="C8" s="2">
         <v>5</v>
       </c>
       <c r="D8" t="s">
+        <v>57</v>
+      </c>
+      <c r="E8" s="3" t="s">
         <v>58</v>
-      </c>
-      <c r="E8" s="3" t="s">
-        <v>59</v>
       </c>
       <c r="F8" s="2" t="s">
         <v>8</v>
@@ -874,7 +879,7 @@
         <v>8</v>
       </c>
       <c r="D11" s="5" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="E11" s="3" t="s">
         <v>31</v>
@@ -955,7 +960,7 @@
         <v>11</v>
       </c>
       <c r="D14" s="5" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E14" s="3" t="s">
         <v>8</v>
@@ -1118,7 +1123,7 @@
         <v>34</v>
       </c>
       <c r="E20" s="3" t="s">
-        <v>8</v>
+        <v>62</v>
       </c>
       <c r="F20" s="3" t="s">
         <v>29</v>
@@ -1211,10 +1216,10 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="J4:J20">
-    <cfRule type="cellIs" dxfId="1" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="10" priority="1" operator="equal">
       <formula>"done"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="0" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="9" priority="2" operator="equal">
       <formula>"done"</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
added put endpoint for User controller, added version field to user class, created userView class for handle new data to update existing user
</commit_message>
<xml_diff>
--- a/TIWPR-PROJEKT-2/RESTdesign.xlsx
+++ b/TIWPR-PROJEKT-2/RESTdesign.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\janbi\Desktop\POLITECHNIKA\2 stopień - SYSTEMY ROZPROSZONE I CHMUROWE\1 semestr\TIwPR\TIwPR-Projekt\TIWPR-PROJEKT-2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D63E3D67-841F-4336-8150-665DAC7EC4DD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{40467DA6-140C-4681-92D5-719F30FEBBA0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="65">
   <si>
     <t>GET</t>
   </si>
@@ -123,9 +123,6 @@
     <t>get list of players by gender</t>
   </si>
   <si>
-    <t>/admin/users</t>
-  </si>
-  <si>
     <t>/games/{gid}</t>
   </si>
   <si>
@@ -138,9 +135,6 @@
     <t>get statistics of games</t>
   </si>
   <si>
-    <t>/admin/users/{id}</t>
-  </si>
-  <si>
     <t>get specific users data</t>
   </si>
   <si>
@@ -214,6 +208,18 @@
   </si>
   <si>
     <t>get token to POST</t>
+  </si>
+  <si>
+    <t>/users/{id}</t>
+  </si>
+  <si>
+    <t>/users</t>
+  </si>
+  <si>
+    <t>only admin can access all users but user can only access his account</t>
+  </si>
+  <si>
+    <t>GET/PUT</t>
   </si>
 </sst>
 </file>
@@ -269,7 +275,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
@@ -294,6 +300,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -642,7 +651,7 @@
   <dimension ref="C3:K29"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="K7" sqref="K7"/>
+      <selection activeCell="J19" sqref="J19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -655,7 +664,7 @@
     <col min="8" max="8" width="13.44140625" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="14.88671875" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="29.88671875" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="11.5546875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="63.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="3" spans="3:11" x14ac:dyDescent="0.3">
@@ -681,7 +690,7 @@
         <v>4</v>
       </c>
       <c r="J3" s="3" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
     </row>
     <row r="4" spans="3:11" x14ac:dyDescent="0.3">
@@ -707,7 +716,7 @@
         <v>8</v>
       </c>
       <c r="J4" s="2" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
     </row>
     <row r="5" spans="3:11" ht="28.8" x14ac:dyDescent="0.3">
@@ -715,7 +724,7 @@
         <v>2</v>
       </c>
       <c r="D5" s="5" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="E5" s="3" t="s">
         <v>24</v>
@@ -733,7 +742,7 @@
         <v>8</v>
       </c>
       <c r="J5" s="2" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="K5" s="2"/>
     </row>
@@ -742,7 +751,7 @@
         <v>3</v>
       </c>
       <c r="D6" s="5" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E6" s="3" t="s">
         <v>13</v>
@@ -769,11 +778,11 @@
         <v>4</v>
       </c>
       <c r="D7" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="E7" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="E7" s="3" t="s">
-        <v>36</v>
-      </c>
       <c r="F7" s="3" t="s">
         <v>8</v>
       </c>
@@ -787,10 +796,10 @@
         <v>8</v>
       </c>
       <c r="J7" s="2" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="K7" s="2" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
     </row>
     <row r="8" spans="3:11" ht="28.8" x14ac:dyDescent="0.3">
@@ -798,10 +807,10 @@
         <v>5</v>
       </c>
       <c r="D8" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="E8" s="3" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="F8" s="2" t="s">
         <v>8</v>
@@ -816,7 +825,7 @@
         <v>8</v>
       </c>
       <c r="J8" s="2" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="K8" s="2"/>
     </row>
@@ -843,7 +852,7 @@
         <v>18</v>
       </c>
       <c r="J9" s="2" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="K9" s="2"/>
     </row>
@@ -855,7 +864,7 @@
         <v>26</v>
       </c>
       <c r="E10" s="7" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="F10" s="7" t="s">
         <v>8</v>
@@ -870,7 +879,7 @@
         <v>9</v>
       </c>
       <c r="J10" s="2" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="K10" s="2"/>
     </row>
@@ -879,7 +888,7 @@
         <v>8</v>
       </c>
       <c r="D11" s="5" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="E11" s="3" t="s">
         <v>31</v>
@@ -897,7 +906,7 @@
         <v>8</v>
       </c>
       <c r="J11" s="2" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="K11" s="2"/>
     </row>
@@ -906,14 +915,14 @@
         <v>9</v>
       </c>
       <c r="D12" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="E12" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="F12" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="E12" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="F12" s="3" t="s">
-        <v>41</v>
-      </c>
       <c r="G12" s="3" t="s">
         <v>8</v>
       </c>
@@ -924,7 +933,7 @@
         <v>8</v>
       </c>
       <c r="J12" s="2" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="K12" s="2"/>
     </row>
@@ -933,25 +942,25 @@
         <v>10</v>
       </c>
       <c r="D13" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="E13" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="F13" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="G13" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="H13" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="E13" s="3" t="s">
-        <v>51</v>
-      </c>
-      <c r="F13" s="3" t="s">
+      <c r="I13" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="J13" s="2" t="s">
         <v>50</v>
-      </c>
-      <c r="G13" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="H13" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="I13" s="3" t="s">
-        <v>45</v>
-      </c>
-      <c r="J13" s="2" t="s">
-        <v>52</v>
       </c>
       <c r="K13" s="2"/>
     </row>
@@ -960,13 +969,13 @@
         <v>11</v>
       </c>
       <c r="D14" s="5" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="E14" s="3" t="s">
         <v>8</v>
       </c>
       <c r="F14" s="3" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="G14" s="3" t="s">
         <v>8</v>
@@ -978,7 +987,7 @@
         <v>8</v>
       </c>
       <c r="J14" s="2" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="K14" s="2"/>
     </row>
@@ -1005,7 +1014,7 @@
         <v>8</v>
       </c>
       <c r="J15" s="2" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="K15" s="2"/>
     </row>
@@ -1032,7 +1041,7 @@
         <v>8</v>
       </c>
       <c r="J16" s="2" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="K16" s="2"/>
     </row>
@@ -1066,7 +1075,7 @@
         <v>16</v>
       </c>
       <c r="D18" s="5" t="s">
-        <v>32</v>
+        <v>62</v>
       </c>
       <c r="E18" s="3" t="s">
         <v>28</v>
@@ -1084,46 +1093,48 @@
         <v>8</v>
       </c>
       <c r="J18" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="K18" s="2"/>
+        <v>47</v>
+      </c>
+      <c r="K18" s="9" t="s">
+        <v>63</v>
+      </c>
     </row>
     <row r="19" spans="3:11" ht="28.8" x14ac:dyDescent="0.3">
       <c r="C19" s="2">
         <v>17</v>
       </c>
       <c r="D19" s="5" t="s">
-        <v>37</v>
+        <v>61</v>
       </c>
       <c r="E19" s="3" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="F19" s="3" t="s">
         <v>8</v>
       </c>
       <c r="G19" s="3" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="H19" s="3" t="s">
         <v>8</v>
       </c>
       <c r="I19" s="3" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="J19" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="K19" s="2"/>
+        <v>64</v>
+      </c>
+      <c r="K19" s="9"/>
     </row>
     <row r="20" spans="3:11" ht="28.8" x14ac:dyDescent="0.3">
       <c r="C20" s="2">
         <v>18</v>
       </c>
       <c r="D20" s="5" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E20" s="3" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="F20" s="3" t="s">
         <v>29</v>
@@ -1138,9 +1149,9 @@
         <v>8</v>
       </c>
       <c r="J20" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="K20" s="2"/>
+        <v>47</v>
+      </c>
+      <c r="K20" s="9"/>
     </row>
     <row r="21" spans="3:11" x14ac:dyDescent="0.3">
       <c r="D21" s="1"/>
@@ -1215,6 +1226,9 @@
       <c r="I29" s="4"/>
     </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="K18:K20"/>
+  </mergeCells>
   <conditionalFormatting sqref="J4:J20">
     <cfRule type="cellIs" dxfId="10" priority="1" operator="equal">
       <formula>"done"</formula>

</xml_diff>

<commit_message>
added patch endpoint for User controller
</commit_message>
<xml_diff>
--- a/TIWPR-PROJEKT-2/RESTdesign.xlsx
+++ b/TIWPR-PROJEKT-2/RESTdesign.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\janbi\Desktop\POLITECHNIKA\2 stopień - SYSTEMY ROZPROSZONE I CHMUROWE\1 semestr\TIwPR\TIwPR-Projekt\TIWPR-PROJEKT-2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{40467DA6-140C-4681-92D5-719F30FEBBA0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A0C3EE04-584E-47E3-B481-A2EE806A8AD7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="65">
   <si>
     <t>GET</t>
   </si>
@@ -219,7 +219,7 @@
     <t>only admin can access all users but user can only access his account</t>
   </si>
   <si>
-    <t>GET/PUT</t>
+    <t>???</t>
   </si>
 </sst>
 </file>
@@ -651,7 +651,7 @@
   <dimension ref="C3:K29"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="J19" sqref="J19"/>
+      <selection activeCell="J18" sqref="J18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1067,7 +1067,9 @@
       <c r="I17" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="J17" s="2"/>
+      <c r="J17" s="2" t="s">
+        <v>64</v>
+      </c>
       <c r="K17" s="2"/>
     </row>
     <row r="18" spans="3:11" ht="43.2" x14ac:dyDescent="0.3">
@@ -1122,7 +1124,7 @@
         <v>46</v>
       </c>
       <c r="J19" s="2" t="s">
-        <v>64</v>
+        <v>47</v>
       </c>
       <c r="K19" s="9"/>
     </row>

</xml_diff>

<commit_message>
moved get all games by player to /player/{id}/games endpoint
</commit_message>
<xml_diff>
--- a/TIWPR-PROJEKT-2/RESTdesign.xlsx
+++ b/TIWPR-PROJEKT-2/RESTdesign.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\janbi\Desktop\POLITECHNIKA\2 stopień - SYSTEMY ROZPROSZONE I CHMUROWE\1 semestr\TIwPR\TIwPR-Projekt\TIWPR-PROJEKT-2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A0C3EE04-584E-47E3-B481-A2EE806A8AD7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5BD0451D-CB06-4BC8-8CB9-6D609DA0519B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3096" yWindow="1824" windowWidth="18024" windowHeight="10260" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Arkusz1" sheetId="1" r:id="rId1"/>
@@ -192,9 +192,6 @@
     <t>Gotowe</t>
   </si>
   <si>
-    <t>/games/players/{id}</t>
-  </si>
-  <si>
     <t>get list of games of the specific player</t>
   </si>
   <si>
@@ -220,6 +217,9 @@
   </si>
   <si>
     <t>???</t>
+  </si>
+  <si>
+    <t>/players/{id}/games</t>
   </si>
 </sst>
 </file>
@@ -310,6 +310,26 @@
   </cellStyles>
   <dxfs count="11">
     <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
@@ -336,26 +356,6 @@
     <dxf>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -370,16 +370,16 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{9A5283A2-05C3-4EF9-8218-D054DDCB57C1}" name="Tabela1" displayName="Tabela1" ref="C3:I20" totalsRowShown="0" headerRowDxfId="8" dataDxfId="7">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{9A5283A2-05C3-4EF9-8218-D054DDCB57C1}" name="Tabela1" displayName="Tabela1" ref="C3:I20" totalsRowShown="0" headerRowDxfId="10" dataDxfId="9">
   <autoFilter ref="C3:I20" xr:uid="{9A5283A2-05C3-4EF9-8218-D054DDCB57C1}"/>
   <tableColumns count="7">
-    <tableColumn id="1" xr3:uid="{B72B4811-05CE-4733-A03C-BB4227A33DA3}" name="LP" dataDxfId="6"/>
-    <tableColumn id="2" xr3:uid="{37F78098-F01B-4E62-B9BB-FD3F43B7744E}" name="endpoint" dataDxfId="5"/>
-    <tableColumn id="3" xr3:uid="{6CE0D21B-2E64-43FB-A8DF-4104A24D4B01}" name="GET" dataDxfId="4"/>
-    <tableColumn id="4" xr3:uid="{C358E3FF-D497-4289-8E7C-EFE8B0BE3375}" name="POST" dataDxfId="3"/>
-    <tableColumn id="5" xr3:uid="{7035C704-2379-47A9-8EED-8B00962C66F6}" name="PUT" dataDxfId="2"/>
-    <tableColumn id="6" xr3:uid="{CAB59842-C01B-47AA-ADB0-BEDA58388076}" name="DELETE" dataDxfId="1"/>
-    <tableColumn id="7" xr3:uid="{55AC5320-F311-42EC-8EE3-50B77673B9EF}" name="PATCH" dataDxfId="0"/>
+    <tableColumn id="1" xr3:uid="{B72B4811-05CE-4733-A03C-BB4227A33DA3}" name="LP" dataDxfId="8"/>
+    <tableColumn id="2" xr3:uid="{37F78098-F01B-4E62-B9BB-FD3F43B7744E}" name="endpoint" dataDxfId="7"/>
+    <tableColumn id="3" xr3:uid="{6CE0D21B-2E64-43FB-A8DF-4104A24D4B01}" name="GET" dataDxfId="6"/>
+    <tableColumn id="4" xr3:uid="{C358E3FF-D497-4289-8E7C-EFE8B0BE3375}" name="POST" dataDxfId="5"/>
+    <tableColumn id="5" xr3:uid="{7035C704-2379-47A9-8EED-8B00962C66F6}" name="PUT" dataDxfId="4"/>
+    <tableColumn id="6" xr3:uid="{CAB59842-C01B-47AA-ADB0-BEDA58388076}" name="DELETE" dataDxfId="3"/>
+    <tableColumn id="7" xr3:uid="{55AC5320-F311-42EC-8EE3-50B77673B9EF}" name="PATCH" dataDxfId="2"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight14" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -650,8 +650,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="C3:K29"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="J18" sqref="J18"/>
+    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -799,110 +799,110 @@
         <v>47</v>
       </c>
       <c r="K7" s="2" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="8" spans="3:11" ht="28.8" x14ac:dyDescent="0.3">
       <c r="C8" s="2">
-        <v>5</v>
-      </c>
-      <c r="D8" t="s">
-        <v>55</v>
+        <v>6</v>
+      </c>
+      <c r="D8" s="5" t="s">
+        <v>7</v>
       </c>
       <c r="E8" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="F8" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="G8" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="H8" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="I8" s="2" t="s">
-        <v>8</v>
+        <v>16</v>
+      </c>
+      <c r="F8" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="G8" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="H8" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="I8" s="3" t="s">
+        <v>18</v>
       </c>
       <c r="J8" s="2" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="K8" s="2"/>
     </row>
     <row r="9" spans="3:11" ht="28.8" x14ac:dyDescent="0.3">
       <c r="C9" s="2">
-        <v>6</v>
-      </c>
-      <c r="D9" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="E9" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="F9" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="G9" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="H9" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="I9" s="3" t="s">
-        <v>18</v>
+      <c r="D9" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="E9" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="F9" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="G9" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="H9" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="I9" s="8" t="s">
+        <v>9</v>
       </c>
       <c r="J9" s="2" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="K9" s="2"/>
     </row>
-    <row r="10" spans="3:11" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="10" spans="3:11" x14ac:dyDescent="0.3">
       <c r="C10" s="2">
-        <v>7</v>
-      </c>
-      <c r="D10" s="6" t="s">
-        <v>26</v>
-      </c>
-      <c r="E10" s="7" t="s">
-        <v>51</v>
-      </c>
-      <c r="F10" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="G10" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="H10" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="I10" s="8" t="s">
-        <v>9</v>
+        <v>8</v>
+      </c>
+      <c r="D10" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="E10" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="F10" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="G10" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="H10" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="I10" s="3" t="s">
+        <v>8</v>
       </c>
       <c r="J10" s="2" t="s">
-        <v>52</v>
+        <v>47</v>
       </c>
       <c r="K10" s="2"/>
     </row>
-    <row r="11" spans="3:11" x14ac:dyDescent="0.3">
+    <row r="11" spans="3:11" ht="28.8" x14ac:dyDescent="0.3">
       <c r="C11" s="2">
-        <v>8</v>
-      </c>
-      <c r="D11" s="5" t="s">
-        <v>58</v>
+        <v>5</v>
+      </c>
+      <c r="D11" t="s">
+        <v>64</v>
       </c>
       <c r="E11" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="F11" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="G11" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="H11" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="I11" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="F11" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="G11" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="H11" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="I11" s="2" t="s">
         <v>8</v>
       </c>
       <c r="J11" s="2" t="s">
@@ -969,7 +969,7 @@
         <v>11</v>
       </c>
       <c r="D14" s="5" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="E14" s="3" t="s">
         <v>8</v>
@@ -1068,7 +1068,7 @@
         <v>8</v>
       </c>
       <c r="J17" s="2" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="K17" s="2"/>
     </row>
@@ -1077,7 +1077,7 @@
         <v>16</v>
       </c>
       <c r="D18" s="5" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="E18" s="3" t="s">
         <v>28</v>
@@ -1098,7 +1098,7 @@
         <v>47</v>
       </c>
       <c r="K18" s="9" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="19" spans="3:11" ht="28.8" x14ac:dyDescent="0.3">
@@ -1106,7 +1106,7 @@
         <v>17</v>
       </c>
       <c r="D19" s="5" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="E19" s="3" t="s">
         <v>36</v>
@@ -1136,7 +1136,7 @@
         <v>33</v>
       </c>
       <c r="E20" s="3" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="F20" s="3" t="s">
         <v>29</v>
@@ -1232,10 +1232,10 @@
     <mergeCell ref="K18:K20"/>
   </mergeCells>
   <conditionalFormatting sqref="J4:J20">
-    <cfRule type="cellIs" dxfId="10" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="1" priority="1" operator="equal">
       <formula>"done"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="9" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="0" priority="2" operator="equal">
       <formula>"done"</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
added version to game class added patch endpoint method to update specific part of a game
</commit_message>
<xml_diff>
--- a/TIWPR-PROJEKT-2/RESTdesign.xlsx
+++ b/TIWPR-PROJEKT-2/RESTdesign.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\janbi\Desktop\POLITECHNIKA\2 stopień - SYSTEMY ROZPROSZONE I CHMUROWE\1 semestr\TIwPR\TIwPR-Projekt\TIWPR-PROJEKT-2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5BD0451D-CB06-4BC8-8CB9-6D609DA0519B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{86A0EF45-EE7A-4D58-AF89-87F164C4A83E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3096" yWindow="1824" windowWidth="18024" windowHeight="10260" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3060" yWindow="1056" windowWidth="18024" windowHeight="10260" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Arkusz1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="66">
   <si>
     <t>GET</t>
   </si>
@@ -220,6 +220,9 @@
   </si>
   <si>
     <t>/players/{id}/games</t>
+  </si>
+  <si>
+    <t>GET/PATCH</t>
   </si>
 </sst>
 </file>
@@ -310,26 +313,6 @@
   </cellStyles>
   <dxfs count="11">
     <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
@@ -356,6 +339,26 @@
     <dxf>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -370,16 +373,16 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{9A5283A2-05C3-4EF9-8218-D054DDCB57C1}" name="Tabela1" displayName="Tabela1" ref="C3:I20" totalsRowShown="0" headerRowDxfId="10" dataDxfId="9">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{9A5283A2-05C3-4EF9-8218-D054DDCB57C1}" name="Tabela1" displayName="Tabela1" ref="C3:I20" totalsRowShown="0" headerRowDxfId="8" dataDxfId="7">
   <autoFilter ref="C3:I20" xr:uid="{9A5283A2-05C3-4EF9-8218-D054DDCB57C1}"/>
   <tableColumns count="7">
-    <tableColumn id="1" xr3:uid="{B72B4811-05CE-4733-A03C-BB4227A33DA3}" name="LP" dataDxfId="8"/>
-    <tableColumn id="2" xr3:uid="{37F78098-F01B-4E62-B9BB-FD3F43B7744E}" name="endpoint" dataDxfId="7"/>
-    <tableColumn id="3" xr3:uid="{6CE0D21B-2E64-43FB-A8DF-4104A24D4B01}" name="GET" dataDxfId="6"/>
-    <tableColumn id="4" xr3:uid="{C358E3FF-D497-4289-8E7C-EFE8B0BE3375}" name="POST" dataDxfId="5"/>
-    <tableColumn id="5" xr3:uid="{7035C704-2379-47A9-8EED-8B00962C66F6}" name="PUT" dataDxfId="4"/>
-    <tableColumn id="6" xr3:uid="{CAB59842-C01B-47AA-ADB0-BEDA58388076}" name="DELETE" dataDxfId="3"/>
-    <tableColumn id="7" xr3:uid="{55AC5320-F311-42EC-8EE3-50B77673B9EF}" name="PATCH" dataDxfId="2"/>
+    <tableColumn id="1" xr3:uid="{B72B4811-05CE-4733-A03C-BB4227A33DA3}" name="LP" dataDxfId="6"/>
+    <tableColumn id="2" xr3:uid="{37F78098-F01B-4E62-B9BB-FD3F43B7744E}" name="endpoint" dataDxfId="5"/>
+    <tableColumn id="3" xr3:uid="{6CE0D21B-2E64-43FB-A8DF-4104A24D4B01}" name="GET" dataDxfId="4"/>
+    <tableColumn id="4" xr3:uid="{C358E3FF-D497-4289-8E7C-EFE8B0BE3375}" name="POST" dataDxfId="3"/>
+    <tableColumn id="5" xr3:uid="{7035C704-2379-47A9-8EED-8B00962C66F6}" name="PUT" dataDxfId="2"/>
+    <tableColumn id="6" xr3:uid="{CAB59842-C01B-47AA-ADB0-BEDA58388076}" name="DELETE" dataDxfId="1"/>
+    <tableColumn id="7" xr3:uid="{55AC5320-F311-42EC-8EE3-50B77673B9EF}" name="PATCH" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight14" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -650,8 +653,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="C3:K29"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="K6" sqref="K6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -769,7 +772,7 @@
         <v>14</v>
       </c>
       <c r="J6" s="2" t="s">
-        <v>0</v>
+        <v>65</v>
       </c>
       <c r="K6" s="2"/>
     </row>
@@ -1232,10 +1235,10 @@
     <mergeCell ref="K18:K20"/>
   </mergeCells>
   <conditionalFormatting sqref="J4:J20">
-    <cfRule type="cellIs" dxfId="1" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="10" priority="1" operator="equal">
       <formula>"done"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="0" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="9" priority="2" operator="equal">
       <formula>"done"</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
added put and patch endpoint for Player and updated build.gradle file
</commit_message>
<xml_diff>
--- a/TIWPR-PROJEKT-2/RESTdesign.xlsx
+++ b/TIWPR-PROJEKT-2/RESTdesign.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\janbi\Desktop\POLITECHNIKA\2 stopień - SYSTEMY ROZPROSZONE I CHMUROWE\1 semestr\TIwPR\TIwPR-Projekt\TIWPR-PROJEKT-2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{86A0EF45-EE7A-4D58-AF89-87F164C4A83E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BBA7A0CA-A70C-4F44-9EB5-F7E74F8A2DFF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3060" yWindow="1056" windowWidth="18024" windowHeight="10260" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Arkusz1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="65">
   <si>
     <t>GET</t>
   </si>
@@ -183,12 +183,6 @@
     <t>get specific user data</t>
   </si>
   <si>
-    <t>get</t>
-  </si>
-  <si>
-    <t>/games?result{WHITE/BLACK/DRAW}</t>
-  </si>
-  <si>
     <t>Gotowe</t>
   </si>
   <si>
@@ -222,7 +216,10 @@
     <t>/players/{id}/games</t>
   </si>
   <si>
-    <t>GET/PATCH</t>
+    <t>/games?result={WHITE/BLACK/DRAW}</t>
+  </si>
+  <si>
+    <t>GET/PUT/PATCH</t>
   </si>
 </sst>
 </file>
@@ -313,6 +310,26 @@
   </cellStyles>
   <dxfs count="11">
     <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
@@ -339,26 +356,6 @@
     <dxf>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -373,16 +370,16 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{9A5283A2-05C3-4EF9-8218-D054DDCB57C1}" name="Tabela1" displayName="Tabela1" ref="C3:I20" totalsRowShown="0" headerRowDxfId="8" dataDxfId="7">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{9A5283A2-05C3-4EF9-8218-D054DDCB57C1}" name="Tabela1" displayName="Tabela1" ref="C3:I20" totalsRowShown="0" headerRowDxfId="10" dataDxfId="9">
   <autoFilter ref="C3:I20" xr:uid="{9A5283A2-05C3-4EF9-8218-D054DDCB57C1}"/>
   <tableColumns count="7">
-    <tableColumn id="1" xr3:uid="{B72B4811-05CE-4733-A03C-BB4227A33DA3}" name="LP" dataDxfId="6"/>
-    <tableColumn id="2" xr3:uid="{37F78098-F01B-4E62-B9BB-FD3F43B7744E}" name="endpoint" dataDxfId="5"/>
-    <tableColumn id="3" xr3:uid="{6CE0D21B-2E64-43FB-A8DF-4104A24D4B01}" name="GET" dataDxfId="4"/>
-    <tableColumn id="4" xr3:uid="{C358E3FF-D497-4289-8E7C-EFE8B0BE3375}" name="POST" dataDxfId="3"/>
-    <tableColumn id="5" xr3:uid="{7035C704-2379-47A9-8EED-8B00962C66F6}" name="PUT" dataDxfId="2"/>
-    <tableColumn id="6" xr3:uid="{CAB59842-C01B-47AA-ADB0-BEDA58388076}" name="DELETE" dataDxfId="1"/>
-    <tableColumn id="7" xr3:uid="{55AC5320-F311-42EC-8EE3-50B77673B9EF}" name="PATCH" dataDxfId="0"/>
+    <tableColumn id="1" xr3:uid="{B72B4811-05CE-4733-A03C-BB4227A33DA3}" name="LP" dataDxfId="8"/>
+    <tableColumn id="2" xr3:uid="{37F78098-F01B-4E62-B9BB-FD3F43B7744E}" name="endpoint" dataDxfId="7"/>
+    <tableColumn id="3" xr3:uid="{6CE0D21B-2E64-43FB-A8DF-4104A24D4B01}" name="GET" dataDxfId="6"/>
+    <tableColumn id="4" xr3:uid="{C358E3FF-D497-4289-8E7C-EFE8B0BE3375}" name="POST" dataDxfId="5"/>
+    <tableColumn id="5" xr3:uid="{7035C704-2379-47A9-8EED-8B00962C66F6}" name="PUT" dataDxfId="4"/>
+    <tableColumn id="6" xr3:uid="{CAB59842-C01B-47AA-ADB0-BEDA58388076}" name="DELETE" dataDxfId="3"/>
+    <tableColumn id="7" xr3:uid="{55AC5320-F311-42EC-8EE3-50B77673B9EF}" name="PATCH" dataDxfId="2"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight14" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -654,13 +651,13 @@
   <dimension ref="C3:K29"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="K6" sqref="K6"/>
+      <selection activeCell="K10" sqref="K10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="3" max="3" width="6.33203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="32.6640625" customWidth="1"/>
+    <col min="4" max="4" width="34.33203125" customWidth="1"/>
     <col min="5" max="5" width="23.88671875" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="14.5546875" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="14.88671875" bestFit="1" customWidth="1"/>
@@ -693,7 +690,7 @@
         <v>4</v>
       </c>
       <c r="J3" s="3" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
     </row>
     <row r="4" spans="3:11" x14ac:dyDescent="0.3">
@@ -727,7 +724,7 @@
         <v>2</v>
       </c>
       <c r="D5" s="5" t="s">
-        <v>53</v>
+        <v>63</v>
       </c>
       <c r="E5" s="3" t="s">
         <v>24</v>
@@ -772,7 +769,7 @@
         <v>14</v>
       </c>
       <c r="J6" s="2" t="s">
-        <v>65</v>
+        <v>47</v>
       </c>
       <c r="K6" s="2"/>
     </row>
@@ -802,10 +799,10 @@
         <v>47</v>
       </c>
       <c r="K7" s="2" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="8" spans="3:11" ht="28.8" x14ac:dyDescent="0.3">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="8" spans="3:11" x14ac:dyDescent="0.3">
       <c r="C8" s="2">
         <v>6</v>
       </c>
@@ -819,16 +816,16 @@
         <v>17</v>
       </c>
       <c r="G8" s="3" t="s">
-        <v>18</v>
+        <v>8</v>
       </c>
       <c r="H8" s="3" t="s">
-        <v>19</v>
+        <v>8</v>
       </c>
       <c r="I8" s="3" t="s">
-        <v>18</v>
+        <v>8</v>
       </c>
       <c r="J8" s="2" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="K8" s="2"/>
     </row>
@@ -845,17 +842,17 @@
       <c r="F9" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="G9" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="H9" s="7" t="s">
-        <v>8</v>
+      <c r="G9" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="H9" s="3" t="s">
+        <v>19</v>
       </c>
       <c r="I9" s="8" t="s">
         <v>9</v>
       </c>
       <c r="J9" s="2" t="s">
-        <v>52</v>
+        <v>64</v>
       </c>
       <c r="K9" s="2"/>
     </row>
@@ -864,7 +861,7 @@
         <v>8</v>
       </c>
       <c r="D10" s="5" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="E10" s="3" t="s">
         <v>31</v>
@@ -891,10 +888,10 @@
         <v>5</v>
       </c>
       <c r="D11" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="E11" s="3" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="F11" s="2" t="s">
         <v>8</v>
@@ -972,7 +969,7 @@
         <v>11</v>
       </c>
       <c r="D14" s="5" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="E14" s="3" t="s">
         <v>8</v>
@@ -1071,7 +1068,7 @@
         <v>8</v>
       </c>
       <c r="J17" s="2" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="K17" s="2"/>
     </row>
@@ -1080,7 +1077,7 @@
         <v>16</v>
       </c>
       <c r="D18" s="5" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="E18" s="3" t="s">
         <v>28</v>
@@ -1101,7 +1098,7 @@
         <v>47</v>
       </c>
       <c r="K18" s="9" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
     </row>
     <row r="19" spans="3:11" ht="28.8" x14ac:dyDescent="0.3">
@@ -1109,7 +1106,7 @@
         <v>17</v>
       </c>
       <c r="D19" s="5" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="E19" s="3" t="s">
         <v>36</v>
@@ -1139,7 +1136,7 @@
         <v>33</v>
       </c>
       <c r="E20" s="3" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="F20" s="3" t="s">
         <v>29</v>
@@ -1235,10 +1232,10 @@
     <mergeCell ref="K18:K20"/>
   </mergeCells>
   <conditionalFormatting sqref="J4:J20">
-    <cfRule type="cellIs" dxfId="10" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="1" priority="1" operator="equal">
       <formula>"done"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="9" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="0" priority="2" operator="equal">
       <formula>"done"</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
added possibility to delete player only if there are no games of player in database
</commit_message>
<xml_diff>
--- a/TIWPR-PROJEKT-2/RESTdesign.xlsx
+++ b/TIWPR-PROJEKT-2/RESTdesign.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\janbi\Desktop\POLITECHNIKA\2 stopień - SYSTEMY ROZPROSZONE I CHMUROWE\1 semestr\TIwPR\TIwPR-Projekt\TIWPR-PROJEKT-2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BBA7A0CA-A70C-4F44-9EB5-F7E74F8A2DFF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BEA65098-EB53-47E3-BED2-EDE302EAD053}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="64">
   <si>
     <t>GET</t>
   </si>
@@ -217,9 +217,6 @@
   </si>
   <si>
     <t>/games?result={WHITE/BLACK/DRAW}</t>
-  </si>
-  <si>
-    <t>GET/PUT/PATCH</t>
   </si>
 </sst>
 </file>
@@ -310,26 +307,6 @@
   </cellStyles>
   <dxfs count="11">
     <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
@@ -356,6 +333,26 @@
     <dxf>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -370,16 +367,16 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{9A5283A2-05C3-4EF9-8218-D054DDCB57C1}" name="Tabela1" displayName="Tabela1" ref="C3:I20" totalsRowShown="0" headerRowDxfId="10" dataDxfId="9">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{9A5283A2-05C3-4EF9-8218-D054DDCB57C1}" name="Tabela1" displayName="Tabela1" ref="C3:I20" totalsRowShown="0" headerRowDxfId="8" dataDxfId="7">
   <autoFilter ref="C3:I20" xr:uid="{9A5283A2-05C3-4EF9-8218-D054DDCB57C1}"/>
   <tableColumns count="7">
-    <tableColumn id="1" xr3:uid="{B72B4811-05CE-4733-A03C-BB4227A33DA3}" name="LP" dataDxfId="8"/>
-    <tableColumn id="2" xr3:uid="{37F78098-F01B-4E62-B9BB-FD3F43B7744E}" name="endpoint" dataDxfId="7"/>
-    <tableColumn id="3" xr3:uid="{6CE0D21B-2E64-43FB-A8DF-4104A24D4B01}" name="GET" dataDxfId="6"/>
-    <tableColumn id="4" xr3:uid="{C358E3FF-D497-4289-8E7C-EFE8B0BE3375}" name="POST" dataDxfId="5"/>
-    <tableColumn id="5" xr3:uid="{7035C704-2379-47A9-8EED-8B00962C66F6}" name="PUT" dataDxfId="4"/>
-    <tableColumn id="6" xr3:uid="{CAB59842-C01B-47AA-ADB0-BEDA58388076}" name="DELETE" dataDxfId="3"/>
-    <tableColumn id="7" xr3:uid="{55AC5320-F311-42EC-8EE3-50B77673B9EF}" name="PATCH" dataDxfId="2"/>
+    <tableColumn id="1" xr3:uid="{B72B4811-05CE-4733-A03C-BB4227A33DA3}" name="LP" dataDxfId="6"/>
+    <tableColumn id="2" xr3:uid="{37F78098-F01B-4E62-B9BB-FD3F43B7744E}" name="endpoint" dataDxfId="5"/>
+    <tableColumn id="3" xr3:uid="{6CE0D21B-2E64-43FB-A8DF-4104A24D4B01}" name="GET" dataDxfId="4"/>
+    <tableColumn id="4" xr3:uid="{C358E3FF-D497-4289-8E7C-EFE8B0BE3375}" name="POST" dataDxfId="3"/>
+    <tableColumn id="5" xr3:uid="{7035C704-2379-47A9-8EED-8B00962C66F6}" name="PUT" dataDxfId="2"/>
+    <tableColumn id="6" xr3:uid="{CAB59842-C01B-47AA-ADB0-BEDA58388076}" name="DELETE" dataDxfId="1"/>
+    <tableColumn id="7" xr3:uid="{55AC5320-F311-42EC-8EE3-50B77673B9EF}" name="PATCH" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight14" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -852,7 +849,7 @@
         <v>9</v>
       </c>
       <c r="J9" s="2" t="s">
-        <v>64</v>
+        <v>47</v>
       </c>
       <c r="K9" s="2"/>
     </row>
@@ -1232,10 +1229,10 @@
     <mergeCell ref="K18:K20"/>
   </mergeCells>
   <conditionalFormatting sqref="J4:J20">
-    <cfRule type="cellIs" dxfId="1" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="10" priority="1" operator="equal">
       <formula>"done"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="0" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="9" priority="2" operator="equal">
       <formula>"done"</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
added possibility to update clubs information with PUT and PATCH methods and added possibility to delete club when no players are in club
</commit_message>
<xml_diff>
--- a/TIWPR-PROJEKT-2/RESTdesign.xlsx
+++ b/TIWPR-PROJEKT-2/RESTdesign.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\janbi\Desktop\POLITECHNIKA\2 stopień - SYSTEMY ROZPROSZONE I CHMUROWE\1 semestr\TIwPR\TIwPR-Projekt\TIWPR-PROJEKT-2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BEA65098-EB53-47E3-BED2-EDE302EAD053}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DCFF0EFE-50F9-4452-9877-444E821A253E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1152" yWindow="1152" windowWidth="17280" windowHeight="8880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Arkusz1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="63">
   <si>
     <t>GET</t>
   </si>
@@ -175,9 +175,6 @@
   </si>
   <si>
     <t>get information of club, and list of players in club</t>
-  </si>
-  <si>
-    <t>GET/POST</t>
   </si>
   <si>
     <t>get specific user data</t>
@@ -647,8 +644,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="C3:K29"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="K10" sqref="K10"/>
+    <sheetView tabSelected="1" topLeftCell="A15" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="K17" sqref="K17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -687,7 +684,7 @@
         <v>4</v>
       </c>
       <c r="J3" s="3" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="4" spans="3:11" x14ac:dyDescent="0.3">
@@ -721,7 +718,7 @@
         <v>2</v>
       </c>
       <c r="D5" s="5" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="E5" s="3" t="s">
         <v>24</v>
@@ -796,7 +793,7 @@
         <v>47</v>
       </c>
       <c r="K7" s="2" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="8" spans="3:11" x14ac:dyDescent="0.3">
@@ -834,7 +831,7 @@
         <v>26</v>
       </c>
       <c r="E9" s="7" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="F9" s="7" t="s">
         <v>8</v>
@@ -858,7 +855,7 @@
         <v>8</v>
       </c>
       <c r="D10" s="5" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E10" s="3" t="s">
         <v>31</v>
@@ -885,10 +882,10 @@
         <v>5</v>
       </c>
       <c r="D11" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="E11" s="3" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="F11" s="2" t="s">
         <v>8</v>
@@ -957,7 +954,7 @@
         <v>43</v>
       </c>
       <c r="J13" s="2" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="K13" s="2"/>
     </row>
@@ -966,7 +963,7 @@
         <v>11</v>
       </c>
       <c r="D14" s="5" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="E14" s="3" t="s">
         <v>8</v>
@@ -1065,7 +1062,7 @@
         <v>8</v>
       </c>
       <c r="J17" s="2" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="K17" s="2"/>
     </row>
@@ -1074,7 +1071,7 @@
         <v>16</v>
       </c>
       <c r="D18" s="5" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="E18" s="3" t="s">
         <v>28</v>
@@ -1095,7 +1092,7 @@
         <v>47</v>
       </c>
       <c r="K18" s="9" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="19" spans="3:11" ht="28.8" x14ac:dyDescent="0.3">
@@ -1103,7 +1100,7 @@
         <v>17</v>
       </c>
       <c r="D19" s="5" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="E19" s="3" t="s">
         <v>36</v>
@@ -1133,7 +1130,7 @@
         <v>33</v>
       </c>
       <c r="E20" s="3" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="F20" s="3" t="s">
         <v>29</v>

</xml_diff>

<commit_message>
added endpoint for getting information about wining for black white and number of game played
</commit_message>
<xml_diff>
--- a/TIWPR-PROJEKT-2/RESTdesign.xlsx
+++ b/TIWPR-PROJEKT-2/RESTdesign.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\janbi\Desktop\POLITECHNIKA\2 stopień - SYSTEMY ROZPROSZONE I CHMUROWE\1 semestr\TIwPR\TIwPR-Projekt\TIWPR-PROJEKT-2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DCFF0EFE-50F9-4452-9877-444E821A253E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{504E0820-E2E2-4E89-A563-E24ADFFD644B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1152" yWindow="1152" windowWidth="17280" windowHeight="8880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Arkusz1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="62">
   <si>
     <t>GET</t>
   </si>
@@ -205,9 +205,6 @@
   </si>
   <si>
     <t>only admin can access all users but user can only access his account</t>
-  </si>
-  <si>
-    <t>???</t>
   </si>
   <si>
     <t>/players/{id}/games</t>
@@ -644,8 +641,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="C3:K29"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A15" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="K17" sqref="K17"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="J18" sqref="J18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -718,7 +715,7 @@
         <v>2</v>
       </c>
       <c r="D5" s="5" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="E5" s="3" t="s">
         <v>24</v>
@@ -882,7 +879,7 @@
         <v>5</v>
       </c>
       <c r="D11" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="E11" s="3" t="s">
         <v>52</v>
@@ -1062,7 +1059,7 @@
         <v>8</v>
       </c>
       <c r="J17" s="2" t="s">
-        <v>60</v>
+        <v>47</v>
       </c>
       <c r="K17" s="2"/>
     </row>

</xml_diff>